<commit_message>
Logger has been fixed.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -28,10 +28,10 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">macro5vv@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acer!1243</t>
+    <t xml:space="preserve">eduardyacenko@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apriorit!1672</t>
   </si>
 </sst>
 </file>
@@ -116,8 +116,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -255,34 +259,34 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="macro5vv@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="eduardyacenko@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>